<commit_message>
update docs and doc folder structure
</commit_message>
<xml_diff>
--- a/docs/metadata-summaries/VRUpdateTaskEphysSummary.xlsx
+++ b/docs/metadata-summaries/VRUpdateTaskEphysSummary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="60">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -172,10 +172,34 @@
     <t xml:space="preserve">Bad movement noise</t>
   </si>
   <si>
-    <t xml:space="preserve">Farther than usual in PFC so check diI</t>
+    <t xml:space="preserve">W190</t>
   </si>
   <si>
-    <t xml:space="preserve">EMG pulses during slow movement</t>
+    <t xml:space="preserve">Y457</t>
+  </si>
+  <si>
+    <t xml:space="preserve">don’t use HPC location was weird</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no licks recorded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not sure about HPC location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some rewards delivered during baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">these got labelled wrong initially</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no spikes, only LFP, something wrong with probe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">careful, might have to exclude 33-64 channels because large fluctuations in raw signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K503</t>
   </si>
 </sst>
 </file>
@@ -289,79 +313,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O109"/>
+  <dimension ref="A1:O189"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C115" activeCellId="0" sqref="C115"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A161" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A187" activeCellId="0" sqref="A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="252" min="15" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="253" min="253" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="254" min="254" style="0" width="7.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="255" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="256" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="257" min="257" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="259" min="258" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="260" min="260" style="0" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="262" min="261" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="263" min="263" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="265" min="264" style="0" width="9.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="266" min="266" style="0" width="8.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="268" min="267" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="269" min="269" style="0" width="7.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="270" min="270" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="508" min="271" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="509" min="509" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="510" min="510" style="0" width="7.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="511" min="511" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="512" min="512" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="513" min="513" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="515" min="514" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="516" min="516" style="0" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="518" min="517" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="519" min="519" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="521" min="520" style="0" width="9.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="522" min="522" style="0" width="8.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="524" min="523" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="525" min="525" style="0" width="7.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="526" min="526" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="764" min="527" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="765" min="765" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="766" min="766" style="0" width="7.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="767" min="767" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="768" min="768" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="769" min="769" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="771" min="770" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="772" min="772" style="0" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="774" min="773" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="775" min="775" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="777" min="776" style="0" width="9.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="778" min="778" style="0" width="8.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="780" min="779" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="781" min="781" style="0" width="7.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="782" min="782" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="783" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1021" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1022" style="0" width="7.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="252" min="15" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="253" min="253" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="254" min="254" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="255" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="256" style="0" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="257" min="257" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="259" min="258" style="0" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="260" min="260" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="262" min="261" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="263" min="263" style="0" width="9.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="265" min="264" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="266" min="266" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="268" min="267" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="269" min="269" style="0" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="270" min="270" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="508" min="271" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="509" min="509" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="510" min="510" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="511" min="511" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="512" min="512" style="0" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="513" min="513" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="515" min="514" style="0" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="516" min="516" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="518" min="517" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="519" min="519" style="0" width="9.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="521" min="520" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="522" min="522" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="524" min="523" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="525" min="525" style="0" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="526" min="526" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="764" min="527" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="765" min="765" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="766" min="766" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="767" min="767" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="768" min="768" style="0" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="769" min="769" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="771" min="770" style="0" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="772" min="772" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="774" min="773" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="775" min="775" style="0" width="9.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="777" min="776" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="778" min="778" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="780" min="779" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="781" min="781" style="0" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="782" min="782" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="783" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1021" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1022" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.83"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +432,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -2173,7 +2197,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>23</v>
       </c>
@@ -2213,11 +2237,8 @@
       <c r="M43" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O43" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>23</v>
       </c>
@@ -2257,11 +2278,8 @@
       <c r="M44" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O44" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>23</v>
       </c>
@@ -2301,9 +2319,6 @@
       <c r="M45" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O45" s="0" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
@@ -3658,7 +3673,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>23</v>
       </c>
@@ -3698,11 +3713,8 @@
       <c r="M79" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O79" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>23</v>
       </c>
@@ -3742,11 +3754,8 @@
       <c r="M80" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O80" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>23</v>
       </c>
@@ -3786,11 +3795,8 @@
       <c r="M81" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O81" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>23</v>
       </c>
@@ -3830,11 +3836,8 @@
       <c r="M82" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O82" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>23</v>
       </c>
@@ -3874,11 +3877,8 @@
       <c r="M83" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O83" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>23</v>
       </c>
@@ -3918,11 +3918,8 @@
       <c r="M84" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O84" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>23</v>
       </c>
@@ -3962,11 +3959,8 @@
       <c r="M85" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O85" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>23</v>
       </c>
@@ -4006,11 +4000,8 @@
       <c r="M86" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O86" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
         <v>23</v>
       </c>
@@ -4050,11 +4041,8 @@
       <c r="M87" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O87" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
         <v>23</v>
       </c>
@@ -4094,11 +4082,8 @@
       <c r="M88" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O88" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>23</v>
       </c>
@@ -4138,11 +4123,8 @@
       <c r="M89" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O89" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>23</v>
       </c>
@@ -4182,11 +4164,8 @@
       <c r="M90" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O90" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>23</v>
       </c>
@@ -4226,11 +4205,8 @@
       <c r="M91" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O91" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>23</v>
       </c>
@@ -4270,11 +4246,8 @@
       <c r="M92" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O92" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>23</v>
       </c>
@@ -4314,11 +4287,8 @@
       <c r="M93" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O93" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>23</v>
       </c>
@@ -4358,9 +4328,6 @@
       <c r="M94" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O94" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
@@ -4402,9 +4369,6 @@
       <c r="M95" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O95" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
@@ -4446,9 +4410,6 @@
       <c r="M96" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O96" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
@@ -4490,9 +4451,6 @@
       <c r="M97" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O97" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
@@ -4534,9 +4492,6 @@
       <c r="M98" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O98" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
@@ -4578,9 +4533,6 @@
       <c r="M99" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O99" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
@@ -4622,9 +4574,6 @@
       <c r="M100" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O100" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
@@ -4666,9 +4615,6 @@
       <c r="M101" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O101" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
@@ -4710,9 +4656,6 @@
       <c r="M102" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O102" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
@@ -4754,9 +4697,6 @@
       <c r="M103" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O103" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
@@ -4798,9 +4738,6 @@
       <c r="M104" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O104" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
@@ -4842,9 +4779,6 @@
       <c r="M105" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O105" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
@@ -4886,9 +4820,6 @@
       <c r="M106" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O106" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
@@ -4930,9 +4861,6 @@
       <c r="M107" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O107" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
@@ -4974,9 +4902,6 @@
       <c r="M108" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O108" s="0" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
@@ -5018,8 +4943,3344 @@
       <c r="M109" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="O109" s="0" t="s">
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B110" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>211104</v>
+      </c>
+      <c r="D110" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E110" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F110" s="0" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="G110" s="0" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H110" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I110" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J110" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K110" s="0" t="s">
         <v>51</v>
+      </c>
+      <c r="L110" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M110" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B111" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C111" s="0" t="n">
+        <v>211104</v>
+      </c>
+      <c r="D111" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E111" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F111" s="0" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="G111" s="0" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H111" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J111" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K111" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L111" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M111" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C112" s="0" t="n">
+        <v>211104</v>
+      </c>
+      <c r="D112" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E112" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F112" s="0" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="G112" s="0" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H112" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I112" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J112" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K112" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L112" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M112" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>211104</v>
+      </c>
+      <c r="D113" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E113" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F113" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G113" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="H113" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I113" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J113" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K113" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="L113" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M113" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B114" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>211104</v>
+      </c>
+      <c r="D114" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E114" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F114" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G114" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="H114" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I114" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J114" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K114" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="L114" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M114" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>211105</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E115" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F115" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="G115" s="0" t="n">
+        <v>1.825</v>
+      </c>
+      <c r="H115" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I115" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J115" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K115" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L115" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M115" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B116" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="C116" s="2" t="n">
+        <v>211105</v>
+      </c>
+      <c r="D116" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E116" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F116" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="G116" s="0" t="n">
+        <v>1.825</v>
+      </c>
+      <c r="H116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J116" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K116" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L116" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M116" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="C117" s="2" t="n">
+        <v>211105</v>
+      </c>
+      <c r="D117" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E117" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F117" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="G117" s="0" t="n">
+        <v>1.825</v>
+      </c>
+      <c r="H117" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I117" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J117" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K117" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L117" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M117" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B118" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="C118" s="2" t="n">
+        <v>211105</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E118" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F118" s="0" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G118" s="0" t="n">
+        <v>2.225</v>
+      </c>
+      <c r="H118" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I118" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J118" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K118" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="L118" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M118" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B119" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="C119" s="2" t="n">
+        <v>211105</v>
+      </c>
+      <c r="D119" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E119" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F119" s="2" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G119" s="2" t="n">
+        <v>2.225</v>
+      </c>
+      <c r="H119" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I119" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J119" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K119" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="L119" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M119" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O119" s="2"/>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B120" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="C120" s="2" t="n">
+        <v>211105</v>
+      </c>
+      <c r="D120" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E120" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F120" s="2" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G120" s="2" t="n">
+        <v>2.225</v>
+      </c>
+      <c r="H120" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I120" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J120" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L120" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M120" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O120" s="2"/>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>211106</v>
+      </c>
+      <c r="D121" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E121" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F121" s="0" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="G121" s="0" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H121" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I121" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J121" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K121" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L121" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M121" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B122" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>211106</v>
+      </c>
+      <c r="D122" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E122" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F122" s="0" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="G122" s="0" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H122" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J122" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K122" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L122" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M122" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B123" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>211106</v>
+      </c>
+      <c r="D123" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E123" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F123" s="0" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="G123" s="0" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H123" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I123" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J123" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K123" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L123" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M123" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>211107</v>
+      </c>
+      <c r="D124" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E124" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F124" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G124" s="0" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="H124" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I124" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J124" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K124" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L124" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M124" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B125" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>211107</v>
+      </c>
+      <c r="D125" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E125" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F125" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G125" s="0" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="H125" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I125" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J125" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K125" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L125" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M125" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B126" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <v>211107</v>
+      </c>
+      <c r="D126" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E126" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F126" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G126" s="0" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="H126" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I126" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J126" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K126" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L126" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M126" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B127" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C127" s="0" t="n">
+        <v>211107</v>
+      </c>
+      <c r="D127" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E127" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F127" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G127" s="0" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H127" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I127" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J127" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K127" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L127" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M127" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O127" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B128" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C128" s="0" t="n">
+        <v>211108</v>
+      </c>
+      <c r="D128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F128" s="0" t="n">
+        <v>2.425</v>
+      </c>
+      <c r="G128" s="0" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="H128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I128" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J128" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K128" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L128" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M128" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B129" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C129" s="0" t="n">
+        <v>211108</v>
+      </c>
+      <c r="D129" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F129" s="0" t="n">
+        <v>2.425</v>
+      </c>
+      <c r="G129" s="0" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="H129" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I129" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J129" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K129" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L129" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M129" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O129" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B130" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C130" s="0" t="n">
+        <v>211108</v>
+      </c>
+      <c r="D130" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E130" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F130" s="0" t="n">
+        <v>2.425</v>
+      </c>
+      <c r="G130" s="0" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="H130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I130" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J130" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K130" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L130" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M130" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O130" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B131" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C131" s="0" t="n">
+        <v>211108</v>
+      </c>
+      <c r="D131" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E131" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F131" s="0" t="n">
+        <v>2.425</v>
+      </c>
+      <c r="G131" s="0" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="H131" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I131" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J131" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K131" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L131" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M131" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O131" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B132" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C132" s="0" t="n">
+        <v>211109</v>
+      </c>
+      <c r="D132" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E132" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F132" s="0" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="G132" s="0" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="H132" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I132" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J132" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K132" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L132" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M132" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O132" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B133" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C133" s="0" t="n">
+        <v>211111</v>
+      </c>
+      <c r="D133" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E133" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F133" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G133" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H133" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I133" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J133" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K133" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L133" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M133" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B134" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C134" s="0" t="n">
+        <v>211111</v>
+      </c>
+      <c r="D134" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E134" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F134" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G134" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I134" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J134" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K134" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L134" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M134" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B135" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C135" s="0" t="n">
+        <v>211111</v>
+      </c>
+      <c r="D135" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E135" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F135" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G135" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H135" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I135" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J135" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K135" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L135" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M135" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B136" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C136" s="0" t="n">
+        <v>211112</v>
+      </c>
+      <c r="D136" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E136" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F136" s="0" t="n">
+        <v>2.275</v>
+      </c>
+      <c r="G136" s="0" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="H136" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I136" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J136" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K136" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L136" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M136" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O136" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B137" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C137" s="0" t="n">
+        <v>211112</v>
+      </c>
+      <c r="D137" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E137" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F137" s="0" t="n">
+        <v>2.275</v>
+      </c>
+      <c r="G137" s="0" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="H137" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J137" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K137" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L137" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M137" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O137" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B138" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C138" s="0" t="n">
+        <v>211113</v>
+      </c>
+      <c r="D138" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E138" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F138" s="0" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="G138" s="0" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="H138" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I138" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J138" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K138" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L138" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M138" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O138" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B139" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C139" s="0" t="n">
+        <v>211113</v>
+      </c>
+      <c r="D139" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E139" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F139" s="0" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="G139" s="0" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="H139" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I139" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J139" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K139" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L139" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M139" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B140" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C140" s="0" t="n">
+        <v>211113</v>
+      </c>
+      <c r="D140" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E140" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F140" s="0" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="G140" s="0" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="H140" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I140" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J140" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K140" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L140" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M140" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B141" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C141" s="0" t="n">
+        <v>211113</v>
+      </c>
+      <c r="D141" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E141" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F141" s="0" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="G141" s="0" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="H141" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I141" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J141" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K141" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L141" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M141" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B142" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C142" s="0" t="n">
+        <v>211114</v>
+      </c>
+      <c r="D142" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E142" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F142" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G142" s="0" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H142" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I142" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J142" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K142" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L142" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M142" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B143" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C143" s="0" t="n">
+        <v>211114</v>
+      </c>
+      <c r="D143" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E143" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F143" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G143" s="0" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H143" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I143" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J143" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K143" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L143" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M143" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B144" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C144" s="0" t="n">
+        <v>211114</v>
+      </c>
+      <c r="D144" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E144" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F144" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G144" s="0" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H144" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I144" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J144" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K144" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L144" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M144" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B145" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C145" s="0" t="n">
+        <v>211114</v>
+      </c>
+      <c r="D145" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E145" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F145" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="G145" s="0" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H145" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I145" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J145" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K145" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L145" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M145" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B146" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C146" s="0" t="n">
+        <v>211114</v>
+      </c>
+      <c r="D146" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E146" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F146" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="G146" s="0" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H146" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I146" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J146" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K146" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L146" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M146" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B147" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C147" s="0" t="n">
+        <v>211114</v>
+      </c>
+      <c r="D147" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E147" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F147" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="G147" s="0" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H147" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I147" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J147" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K147" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L147" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M147" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B148" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C148" s="0" t="n">
+        <v>211115</v>
+      </c>
+      <c r="D148" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E148" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F148" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G148" s="0" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H148" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I148" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J148" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="K148" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="L148" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M148" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B149" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C149" s="0" t="n">
+        <v>211115</v>
+      </c>
+      <c r="D149" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E149" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F149" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G149" s="0" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H149" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I149" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J149" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="K149" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="L149" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M149" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B150" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C150" s="0" t="n">
+        <v>211115</v>
+      </c>
+      <c r="D150" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E150" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F150" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G150" s="0" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H150" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I150" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J150" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="K150" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="L150" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M150" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B151" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C151" s="0" t="n">
+        <v>211116</v>
+      </c>
+      <c r="D151" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E151" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F151" s="0" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="G151" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H151" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I151" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J151" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K151" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L151" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M151" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B152" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C152" s="0" t="n">
+        <v>211116</v>
+      </c>
+      <c r="D152" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E152" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F152" s="0" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="G152" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H152" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I152" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J152" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K152" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L152" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M152" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B153" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C153" s="0" t="n">
+        <v>211116</v>
+      </c>
+      <c r="D153" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E153" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F153" s="0" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="G153" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H153" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I153" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J153" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K153" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L153" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M153" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B154" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C154" s="0" t="n">
+        <v>211116</v>
+      </c>
+      <c r="D154" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E154" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F154" s="0" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="G154" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H154" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I154" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J154" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K154" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L154" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M154" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B155" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C155" s="0" t="n">
+        <v>211116</v>
+      </c>
+      <c r="D155" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E155" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F155" s="0" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="G155" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H155" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I155" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J155" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K155" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L155" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M155" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B156" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C156" s="0" t="n">
+        <v>211116</v>
+      </c>
+      <c r="D156" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E156" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F156" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G156" s="0" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H156" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I156" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J156" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K156" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L156" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M156" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B157" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C157" s="0" t="n">
+        <v>211116</v>
+      </c>
+      <c r="D157" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E157" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F157" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G157" s="0" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H157" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I157" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J157" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K157" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L157" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M157" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B158" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C158" s="0" t="n">
+        <v>211117</v>
+      </c>
+      <c r="D158" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E158" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F158" s="0" t="n">
+        <v>2.175</v>
+      </c>
+      <c r="G158" s="0" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H158" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I158" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J158" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K158" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L158" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M158" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B159" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C159" s="0" t="n">
+        <v>211117</v>
+      </c>
+      <c r="D159" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E159" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F159" s="0" t="n">
+        <v>2.175</v>
+      </c>
+      <c r="G159" s="0" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H159" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I159" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J159" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K159" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L159" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M159" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O159" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B160" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C160" s="0" t="n">
+        <v>211118</v>
+      </c>
+      <c r="D160" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E160" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F160" s="0" t="n">
+        <v>2.225</v>
+      </c>
+      <c r="G160" s="0" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="H160" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I160" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J160" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K160" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L160" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O160" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B161" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C161" s="0" t="n">
+        <v>211118</v>
+      </c>
+      <c r="D161" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E161" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F161" s="0" t="n">
+        <v>2.225</v>
+      </c>
+      <c r="G161" s="0" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="H161" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I161" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J161" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K161" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L161" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O161" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B162" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C162" s="0" t="n">
+        <v>211118</v>
+      </c>
+      <c r="D162" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E162" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F162" s="0" t="n">
+        <v>2.225</v>
+      </c>
+      <c r="G162" s="0" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="H162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J162" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K162" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L162" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M162" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O162" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B163" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C163" s="0" t="n">
+        <v>211118</v>
+      </c>
+      <c r="D163" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E163" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F163" s="0" t="n">
+        <v>2.225</v>
+      </c>
+      <c r="G163" s="0" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="H163" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I163" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J163" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K163" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L163" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M163" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O163" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B164" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C164" s="0" t="n">
+        <v>211118</v>
+      </c>
+      <c r="D164" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E164" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F164" s="0" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="G164" s="0" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H164" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I164" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J164" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K164" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L164" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M164" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B165" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C165" s="0" t="n">
+        <v>211118</v>
+      </c>
+      <c r="D165" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E165" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F165" s="0" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="G165" s="0" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H165" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I165" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J165" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K165" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L165" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M165" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B166" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C166" s="0" t="n">
+        <v>211119</v>
+      </c>
+      <c r="D166" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E166" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F166" s="0" t="n">
+        <v>2.175</v>
+      </c>
+      <c r="G166" s="0" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H166" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I166" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J166" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K166" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L166" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M166" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O166" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B167" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C167" s="0" t="n">
+        <v>211119</v>
+      </c>
+      <c r="D167" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E167" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F167" s="0" t="n">
+        <v>2.175</v>
+      </c>
+      <c r="G167" s="0" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I167" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J167" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K167" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L167" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M167" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O167" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B168" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C168" s="0" t="n">
+        <v>211119</v>
+      </c>
+      <c r="D168" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E168" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F168" s="0" t="n">
+        <v>2.175</v>
+      </c>
+      <c r="G168" s="0" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H168" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I168" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J168" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K168" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L168" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M168" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O168" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B169" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C169" s="0" t="n">
+        <v>211119</v>
+      </c>
+      <c r="D169" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E169" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F169" s="0" t="n">
+        <v>2.325</v>
+      </c>
+      <c r="G169" s="0" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H169" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I169" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J169" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K169" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L169" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M169" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B170" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C170" s="0" t="n">
+        <v>211119</v>
+      </c>
+      <c r="D170" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E170" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F170" s="0" t="n">
+        <v>2.325</v>
+      </c>
+      <c r="G170" s="0" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I170" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J170" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K170" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L170" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M170" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B171" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C171" s="0" t="n">
+        <v>211119</v>
+      </c>
+      <c r="D171" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E171" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F171" s="0" t="n">
+        <v>2.325</v>
+      </c>
+      <c r="G171" s="0" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H171" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I171" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J171" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K171" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L171" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M171" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B172" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C172" s="0" t="n">
+        <v>211120</v>
+      </c>
+      <c r="D172" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E172" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F172" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G172" s="0" t="n">
+        <v>1.825</v>
+      </c>
+      <c r="H172" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I172" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J172" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K172" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L172" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M172" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B173" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C173" s="0" t="n">
+        <v>211120</v>
+      </c>
+      <c r="D173" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E173" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F173" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G173" s="0" t="n">
+        <v>1.825</v>
+      </c>
+      <c r="H173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I173" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J173" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K173" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L173" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M173" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B174" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C174" s="0" t="n">
+        <v>211120</v>
+      </c>
+      <c r="D174" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E174" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F174" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G174" s="0" t="n">
+        <v>1.825</v>
+      </c>
+      <c r="H174" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I174" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J174" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K174" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L174" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M174" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B175" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C175" s="0" t="n">
+        <v>211121</v>
+      </c>
+      <c r="D175" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E175" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F175" s="0" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="G175" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H175" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I175" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J175" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K175" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="L175" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M175" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O175" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B176" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C176" s="0" t="n">
+        <v>211121</v>
+      </c>
+      <c r="D176" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E176" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F176" s="0" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="G176" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H176" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I176" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J176" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K176" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="L176" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M176" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O176" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B177" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C177" s="0" t="n">
+        <v>211121</v>
+      </c>
+      <c r="D177" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E177" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F177" s="0" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="G177" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H177" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I177" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J177" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K177" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="L177" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M177" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O177" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B178" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C178" s="0" t="n">
+        <v>211122</v>
+      </c>
+      <c r="D178" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E178" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F178" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G178" s="0" t="n">
+        <v>2.125</v>
+      </c>
+      <c r="H178" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I178" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J178" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K178" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L178" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M178" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B179" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C179" s="0" t="n">
+        <v>211122</v>
+      </c>
+      <c r="D179" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E179" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F179" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G179" s="0" t="n">
+        <v>2.125</v>
+      </c>
+      <c r="H179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I179" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J179" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K179" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L179" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M179" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B180" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C180" s="0" t="n">
+        <v>211122</v>
+      </c>
+      <c r="D180" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E180" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F180" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G180" s="0" t="n">
+        <v>2.125</v>
+      </c>
+      <c r="H180" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I180" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J180" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K180" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L180" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M180" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B181" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C181" s="0" t="n">
+        <v>211122</v>
+      </c>
+      <c r="D181" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E181" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F181" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G181" s="0" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H181" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I181" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J181" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K181" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L181" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M181" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B182" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C182" s="0" t="n">
+        <v>211122</v>
+      </c>
+      <c r="D182" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E182" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F182" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G182" s="0" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I182" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J182" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K182" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L182" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M182" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B183" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C183" s="0" t="n">
+        <v>211122</v>
+      </c>
+      <c r="D183" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E183" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F183" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G183" s="0" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H183" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I183" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J183" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K183" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L183" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M183" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B184" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C184" s="0" t="n">
+        <v>211123</v>
+      </c>
+      <c r="D184" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E184" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F184" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G184" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H184" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I184" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J184" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K184" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L184" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M184" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B185" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C185" s="0" t="n">
+        <v>211123</v>
+      </c>
+      <c r="D185" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E185" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F185" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G185" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H185" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I185" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J185" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K185" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L185" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M185" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B186" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C186" s="0" t="n">
+        <v>211123</v>
+      </c>
+      <c r="D186" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E186" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F186" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G186" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H186" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I186" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J186" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K186" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L186" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M186" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B187" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C187" s="0" t="n">
+        <v>211123</v>
+      </c>
+      <c r="D187" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E187" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F187" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G187" s="0" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H187" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I187" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J187" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K187" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L187" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M187" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B188" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C188" s="0" t="n">
+        <v>211123</v>
+      </c>
+      <c r="D188" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E188" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F188" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G188" s="0" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H188" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I188" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J188" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K188" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L188" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M188" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B189" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C189" s="0" t="n">
+        <v>211123</v>
+      </c>
+      <c r="D189" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E189" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F189" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G189" s="0" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H189" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I189" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J189" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K189" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L189" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="M189" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>